<commit_message>
add image to product
</commit_message>
<xml_diff>
--- a/public/files/example.xlsx
+++ b/public/files/example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59ec75f4eb9d40eb/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\Tes Kerja\BPH Migas\simple-web-store\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{FE936C65-D35D-486A-974C-7C9D27323DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21A14653-5392-4A87-9810-5D188A8B5785}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1CC4C8-B761-4B6C-BEE8-3CBC5CF2CE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{08B8E078-C736-4586-8580-D1C60C912E4A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>example name</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>https://placehold.co/600x400/EEE/31343C</t>
   </si>
 </sst>
 </file>
@@ -96,10 +102,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041D0EF3-A94D-4B96-AEEC-CC7A303C8321}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +412,7 @@
     <col min="3" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,8 +425,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -436,6 +441,9 @@
       </c>
       <c r="D2" s="1">
         <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>